<commit_message>
重新整理了下Wigner Matrix construction recurrence
</commit_message>
<xml_diff>
--- a/球谐光照/SH Rotation/Wigner matrix recurrence.xlsx
+++ b/球谐光照/SH Rotation/Wigner matrix recurrence.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="7">
   <si>
     <t>(L,L)</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -225,12 +225,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,7 +241,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -549,9 +543,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
-      <c r="I1" s="19">
-        <v>0</v>
-      </c>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -564,9 +556,7 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="I2" s="20">
-        <v>0</v>
-      </c>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -579,9 +569,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="20">
-        <v>0</v>
-      </c>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
@@ -594,15 +582,13 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="20">
-        <v>0</v>
-      </c>
+      <c r="I4" s="17"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>0</v>
+      <c r="A5" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -618,9 +604,7 @@
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
-        <v>0</v>
-      </c>
+      <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -635,9 +619,7 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>0</v>
-      </c>
+      <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -652,9 +634,7 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>0</v>
-      </c>
+      <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -669,9 +649,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
-        <v>0</v>
-      </c>
+      <c r="A9" s="15"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -979,19 +957,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -1004,9 +980,7 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="I2" s="20">
-        <v>0</v>
-      </c>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -1019,9 +993,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="20">
-        <v>0</v>
-      </c>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
@@ -1034,13 +1006,11 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="20">
-        <v>0</v>
-      </c>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>0</v>
+      <c r="A5" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1054,9 +1024,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
-        <v>0</v>
-      </c>
+      <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -1069,9 +1037,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>0</v>
-      </c>
+      <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -1084,9 +1050,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>0</v>
-      </c>
+      <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -1099,12 +1063,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22">
-        <v>0</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1133,19 +1095,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22">
-        <v>0</v>
-      </c>
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -1163,18 +1123,10 @@
       <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24">
-        <v>0</v>
-      </c>
-      <c r="G2" s="24">
-        <v>0</v>
-      </c>
-      <c r="H2" s="24">
-        <v>0</v>
-      </c>
-      <c r="I2" s="20">
-        <v>0</v>
-      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -1192,18 +1144,10 @@
       <c r="E3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="24">
-        <v>0</v>
-      </c>
-      <c r="G3" s="24">
-        <v>0</v>
-      </c>
-      <c r="H3" s="24">
-        <v>0</v>
-      </c>
-      <c r="I3" s="20">
-        <v>0</v>
-      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
@@ -1221,22 +1165,14 @@
       <c r="E4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="24">
-        <v>0</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0</v>
-      </c>
-      <c r="I4" s="20">
-        <v>0</v>
-      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>0</v>
+      <c r="A5" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>5</v>
@@ -1264,18 +1200,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
-        <v>0</v>
-      </c>
-      <c r="B6" s="26">
-        <v>0</v>
-      </c>
-      <c r="C6" s="26">
-        <v>0</v>
-      </c>
-      <c r="D6" s="26">
-        <v>0</v>
-      </c>
+      <c r="A6" s="25"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1293,18 +1221,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>0</v>
-      </c>
-      <c r="B7" s="26">
-        <v>0</v>
-      </c>
-      <c r="C7" s="26">
-        <v>0</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
+      <c r="A7" s="25"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1322,18 +1242,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>0</v>
-      </c>
-      <c r="B8" s="26">
-        <v>0</v>
-      </c>
-      <c r="C8" s="26">
-        <v>0</v>
-      </c>
-      <c r="D8" s="26">
-        <v>0</v>
-      </c>
+      <c r="A8" s="25"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="13" t="s">
         <v>4</v>
       </c>
@@ -1351,12 +1263,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22">
-        <v>0</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1376,7 +1286,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1385,16 +1295,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="3">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3">
+        <v>0</v>
+      </c>
       <c r="I1" s="3">
         <v>0</v>
       </c>
@@ -1487,8 +1403,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>0</v>
+      <c r="A5" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>5</v>
@@ -1502,16 +1418,16 @@
       <c r="E5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="25">
-        <v>0</v>
-      </c>
-      <c r="G5" s="25">
-        <v>0</v>
-      </c>
-      <c r="H5" s="25">
-        <v>0</v>
-      </c>
-      <c r="I5" s="25">
+      <c r="F5" s="23">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0</v>
+      </c>
+      <c r="I5" s="23">
         <v>0</v>
       </c>
     </row>
@@ -1519,16 +1435,16 @@
       <c r="A6" s="3">
         <v>0</v>
       </c>
-      <c r="B6" s="25">
-        <v>0</v>
-      </c>
-      <c r="C6" s="25">
-        <v>0</v>
-      </c>
-      <c r="D6" s="25">
-        <v>0</v>
-      </c>
-      <c r="E6" s="25">
+      <c r="B6" s="23">
+        <v>0</v>
+      </c>
+      <c r="C6" s="23">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0</v>
+      </c>
+      <c r="E6" s="23">
         <v>0</v>
       </c>
       <c r="F6" s="13" t="s">
@@ -1548,16 +1464,16 @@
       <c r="A7" s="3">
         <v>0</v>
       </c>
-      <c r="B7" s="25">
-        <v>0</v>
-      </c>
-      <c r="C7" s="25">
-        <v>0</v>
-      </c>
-      <c r="D7" s="25">
-        <v>0</v>
-      </c>
-      <c r="E7" s="25">
+      <c r="B7" s="23">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0</v>
+      </c>
+      <c r="E7" s="23">
         <v>0</v>
       </c>
       <c r="F7" s="13" t="s">
@@ -1577,16 +1493,16 @@
       <c r="A8" s="3">
         <v>0</v>
       </c>
-      <c r="B8" s="25">
-        <v>0</v>
-      </c>
-      <c r="C8" s="25">
-        <v>0</v>
-      </c>
-      <c r="D8" s="25">
-        <v>0</v>
-      </c>
-      <c r="E8" s="25">
+      <c r="B8" s="23">
+        <v>0</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
         <v>0</v>
       </c>
       <c r="F8" s="13" t="s">
@@ -1606,10 +1522,18 @@
       <c r="A9" s="3">
         <v>0</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>

</xml_diff>